<commit_message>
Regenerate Excel spreadsheet via openpyxl
No content changes; file was re-saved during website generation process.

https://claude.ai/code/session_015zL8AEuvfUGA59cjgfEpnA
</commit_message>
<xml_diff>
--- a/Green_Star_Buildings_v1.1_Submission_Questions.xlsx
+++ b/Green_Star_Buildings_v1.1_Submission_Questions.xlsx
@@ -1,56 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Industry Development" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Construction" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Verification and Handover" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Resource Mgmt" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Procurement" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Structure" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Envelope" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Systems" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Responsible Finishes" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Impacts Disclosure" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clean Air" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Light Quality" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acoustic Comfort" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Exposure to Toxins" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Amenity and Comfort" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connection to Nature" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Climate Resilience" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operations Resilience" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Community Resilience" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Heat Resilience" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grid Resilience" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy Source" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy Use" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upfront Carbon Reduction" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upfront Carbon Compensation" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Refrigerant Systems Impacts" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Low-Emissions Transport" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design for Circularity" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Water Use" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Movement and Place" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enjoyable Places" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contribution to Place" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Culture Heritage Identity" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inclusive Construction" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="First Nations Inclusion" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Procurement Workforce Inclusion" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Design for Equity" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Impacts to Nature" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Biodiversity Enhancement" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nature Connectivity" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nature Stewardship" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Waterway Protection" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Market Transformation" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Leadership Challenges" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="Industry Development" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Responsible Construction" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Verification and Handover" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Responsible Resource Mgmt" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Responsible Procurement" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Responsible Structure" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Responsible Envelope" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Responsible Systems" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Responsible Finishes" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Impacts Disclosure" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Clean Air" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Light Quality" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Acoustic Comfort" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Exposure to Toxins" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Amenity and Comfort" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Connection to Nature" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Climate Resilience" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Operations Resilience" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Community Resilience" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Heat Resilience" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Grid Resilience" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Energy Source" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Energy Use" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Upfront Carbon Reduction" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Upfront Carbon Compensation" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Refrigerant Systems Impacts" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Low-Emissions Transport" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Design for Circularity" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Water Use" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Movement and Place" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Enjoyable Places" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Contribution to Place" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Culture Heritage Identity" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Inclusive Construction" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="First Nations Inclusion" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="Procurement Workforce Inclusion" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="Design for Equity" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="Impacts to Nature" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="Biodiversity Enhancement" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="Nature Connectivity" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="Nature Stewardship" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="Waterway Protection" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="Market Transformation" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="Leadership Challenges" sheetId="44" state="visible" r:id="rId44"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>